<commit_message>
carga grua, personal, tipopersonal e inicio de colectivos
</commit_message>
<xml_diff>
--- a/Excel/Carga DB Postgres/Playa - CARGADO.xlsx
+++ b/Excel/Carga DB Postgres/Playa - CARGADO.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="18915" windowHeight="7995"/>
+    <workbookView xWindow="120" yWindow="48" windowWidth="18912" windowHeight="7992"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -365,7 +365,10 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="2" max="2" width="14.44140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -402,7 +405,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -414,7 +417,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>